<commit_message>
Add president raw chart overlay, caption, and higher-contrast light theme
</commit_message>
<xml_diff>
--- a/codex_handoff_pack/outputs/forecast_next_week.xlsx
+++ b/codex_handoff_pack/outputs/forecast_next_week.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,31 @@
           <t>rmse</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>pred_sd</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>pred_lo_80</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>pred_hi_80</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>exog_approval</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -457,10 +482,29 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>44.04890285258966</v>
+        <v>44.3382262630215</v>
       </c>
       <c r="C2" t="n">
-        <v>1.59139647135574</v>
+        <v>1.782502371047188</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.477564416905923</v>
+      </c>
+      <c r="E2" t="n">
+        <v>42.44465127134272</v>
+      </c>
+      <c r="F2" t="n">
+        <v>46.23180125470029</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ssm</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -470,10 +514,29 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>36.70307273299944</v>
+        <v>35.97098622709436</v>
       </c>
       <c r="C3" t="n">
-        <v>2.144301275746056</v>
+        <v>2.848716697536143</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2.635585571360043</v>
+      </c>
+      <c r="E3" t="n">
+        <v>32.59334741199113</v>
+      </c>
+      <c r="F3" t="n">
+        <v>39.34862504219758</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ssm</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -483,10 +546,29 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2.774446351258108</v>
+        <v>2.723575158728821</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5317315905115642</v>
+        <v>0.6925965779035405</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.6317443829491085</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.913962155736383</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.533188161721258</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ssm</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -496,10 +578,29 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.409505631613268</v>
+        <v>1.276709263833665</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2486437043494172</v>
+        <v>0.3026656212035301</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.2691008467461636</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.9318426523967411</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.621575875270588</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ssm</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -509,10 +610,29 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.860006116568211</v>
+        <v>3.134954891566468</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6801730732212364</v>
+        <v>0.6201143687290629</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.6546931947237548</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.295931802916845</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.973977980216092</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>ssm</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -522,10 +642,29 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.399962351078833</v>
+        <v>2.049992320667111</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9061998261105985</v>
+        <v>0.7315696826819685</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.7002957758226334</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.152527172817345</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2.947457468516877</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>ssm</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -536,10 +675,29 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8.661977042547171</v>
+        <v>9.179588433454013</v>
       </c>
       <c r="C8" t="n">
-        <v>1.330183043987214</v>
+        <v>1.551212647681675</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.478988215955746</v>
+      </c>
+      <c r="E8" t="n">
+        <v>7.284188769873912</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11.07498809703412</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>ssm</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -550,10 +708,29 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.123977482460778</v>
+        <v>1.15661508591859</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2844372422059417</v>
+        <v>0.2959424388078578</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.2571016066550879</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.8271261194057304</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.48610405243145</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>ssm</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>